<commit_message>
fix: update poi import example - this commit updates the poi import example to match the new format and change the poi_types and themes column to use the identifier instead of the name
</commit_message>
<xml_diff>
--- a/public/importer-examples/import-poi-example.xlsx
+++ b/public/importer-examples/import-poi-example.xlsx
@@ -64,10 +64,10 @@
     <t>Azienda Agricola Biologica Alloggio Turistico</t>
   </si>
   <si>
-    <t>Borgo</t>
-  </si>
-  <si>
-    <t>Ciaspole</t>
+    <t>tower</t>
+  </si>
+  <si>
+    <t>ridge-route</t>
   </si>
   <si>
     <t>42.16824</t>
@@ -103,10 +103,10 @@
     <t>Rifugio di Montagna</t>
   </si>
   <si>
-    <t>Rifugio</t>
-  </si>
-  <si>
-    <t>Piccola Cassia</t>
+    <t>beach</t>
+  </si>
+  <si>
+    <t>nature-route</t>
   </si>
   <si>
     <t>42.16652</t>
@@ -142,10 +142,10 @@
     <t>Campeggio</t>
   </si>
   <si>
-    <t>Camping</t>
-  </si>
-  <si>
-    <t>Ciclovie</t>
+    <t>religion</t>
+  </si>
+  <si>
+    <t>sentiero-ducati</t>
   </si>
   <si>
     <t>42.16340</t>
@@ -883,7 +883,7 @@
     <col min="14" max="14" style="26" width="14.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="30" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="28.5" customFormat="1" s="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -927,7 +927,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="60" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="57" customFormat="1" s="1">
       <c r="A2" s="5">
         <v>399</v>
       </c>
@@ -963,7 +963,7 @@
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="33" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="31.5" customFormat="1" s="1">
       <c r="A3" s="9">
         <v>400</v>
       </c>
@@ -999,7 +999,7 @@
         <v>31</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="33" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="31.5" customFormat="1" s="1">
       <c r="A4" s="9">
         <v>402</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>40</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A5" s="13"/>
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
@@ -1051,7 +1051,7 @@
       <c r="M5" s="14"/>
       <c r="N5" s="16"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A6" s="17"/>
       <c r="B6" s="18"/>
       <c r="C6" s="18"/>
@@ -1067,7 +1067,7 @@
       <c r="M6" s="18"/>
       <c r="N6" s="20"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A7" s="17"/>
       <c r="B7" s="18"/>
       <c r="C7" s="18"/>
@@ -1083,7 +1083,7 @@
       <c r="M7" s="18"/>
       <c r="N7" s="20"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A8" s="17"/>
       <c r="B8" s="18"/>
       <c r="C8" s="18"/>
@@ -1099,7 +1099,7 @@
       <c r="M8" s="18"/>
       <c r="N8" s="20"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A9" s="21"/>
       <c r="B9" s="22"/>
       <c r="C9" s="22"/>

</xml_diff>